<commit_message>
Update industrial biomass extension.
</commit_message>
<xml_diff>
--- a/input/extention/sector_percents_start.xlsx
+++ b/input/extention/sector_percents_start.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25600" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14080" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="coal" sheetId="1" r:id="rId1"/>
     <sheet name="natural_gas" sheetId="2" r:id="rId2"/>
     <sheet name="petroleum" sheetId="3" r:id="rId3"/>
+    <sheet name="other_biomass" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="36">
   <si>
     <t>ext_sector</t>
   </si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t>1A3eii_Other-transp</t>
+  </si>
+  <si>
+    <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>X1850</t>
   </si>
 </sst>
 </file>
@@ -171,17 +178,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1178,7 +1193,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1497,6 +1512,135 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>